<commit_message>
Big updates to MSC
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/MSC/Data/MSC Template v10.xlsx
+++ b/Projects/CCBOTTLERSUS/MSC/Data/MSC Template v10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$30</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$F$30</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$F$30</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$Q$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -416,6 +417,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -436,18 +438,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -455,6 +460,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <strike val="true"/>
@@ -462,6 +468,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -524,7 +531,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -593,24 +600,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -661,24 +656,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -776,7 +759,7 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -786,14 +769,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.60740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="44.6851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="38.4148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="46.1555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="45.862962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="39.3925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="47.3296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="32.9259259259259"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1404,35 +1387,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:11"/>
+  <dimension ref="A1:AMI11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="36.5518518518518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="37.4333333333333"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="11" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="19.1555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="22.7074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="15.8962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="10" width="16.6851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="18.7555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="10" width="21.2259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="10" width="23.0037037037037"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="10" width="25.2740740740741"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="10" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="10" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="10" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="10" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="12" width="56.5407407407407"/>
-    <col collapsed="false" hidden="false" max="1023" min="19" style="12" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="10" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="10" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="10" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="10" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="10" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="10" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="10" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="10" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="12" width="57.9148148148148"/>
+    <col collapsed="false" hidden="false" max="1023" min="19" style="12" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="30.9666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,38 +2490,33 @@
       <c r="C2" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17" t="n">
+      <c r="N2" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="17"/>
       <c r="R2" s="0"/>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
@@ -3554,36 +3532,28 @@
         <f aca="false">VLOOKUP(A3,KPIs!B:C,2,0)</f>
         <v>43497</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>76</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17" t="n">
+      <c r="O3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="12" t="s">
         <v>81</v>
       </c>
       <c r="S3" s="0"/>
@@ -4592,7 +4562,7 @@
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
     </row>
-    <row r="4" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
@@ -4600,35 +4570,24 @@
         <f aca="false">VLOOKUP(A4,KPIs!B:C,2,0)</f>
         <v>43498</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="10" t="s">
         <v>82</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17" t="n">
+      <c r="M4" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="19"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
@@ -4636,30 +4595,19 @@
         <f aca="false">VLOOKUP(A5,KPIs!B:C,2,0)</f>
         <v>43500</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="10" t="s">
         <v>83</v>
       </c>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17" t="n">
+      <c r="M5" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" s="18" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
@@ -4667,32 +4615,21 @@
         <f aca="false">VLOOKUP(A6,KPIs!B:C,2,0)</f>
         <v>43501</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17" t="n">
+      <c r="M6" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
@@ -4705,36 +4642,30 @@
       <c r="C7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17" t="n">
+      <c r="N7" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
@@ -4744,27 +4675,21 @@
         <f aca="false">VLOOKUP(A8,KPIs!B:C,2,0)</f>
         <v>43556</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
-      <c r="M8" s="17" t="n">
+      <c r="M8" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
@@ -4774,31 +4699,21 @@
         <f aca="false">VLOOKUP(A9,KPIs!B:C,2,0)</f>
         <v>43588</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="10" t="s">
         <v>86</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17" t="n">
+      <c r="M9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
@@ -4808,31 +4723,21 @@
         <f aca="false">VLOOKUP(A10,KPIs!B:C,2,0)</f>
         <v>43589</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="10" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17" t="n">
+      <c r="M10" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
@@ -4842,31 +4747,21 @@
         <f aca="false">VLOOKUP(A11,KPIs!B:C,2,0)</f>
         <v>43590</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="10" t="s">
         <v>84</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17" t="n">
+      <c r="M11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4891,133 +4786,134 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="44.6851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="4.11481481481482"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="12.537037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="18" width="12.537037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="18" width="29.3259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="23" width="29.3259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="24" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="18" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="18" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="18" width="19.7407407407407"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="18" width="56.5407407407407"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="18" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="45.862962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="4.11481481481482"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="24.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="19" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="21" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="12" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="12" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="12" width="57.9148148148148"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="12" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="30.9666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="26" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="B2" s="11" t="n">
         <v>43472</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="0"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
-      <c r="I2" s="30"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="0"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="20" t="s">
         <v>93</v>
       </c>
       <c r="M2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="11" t="n">
         <v>43473</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>95</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="I3" s="30" t="n">
+      <c r="I3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="J3" s="0"/>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="20" t="s">
         <v>93</v>
       </c>
       <c r="M3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="11" t="n">
         <f aca="false">VLOOKUP(A4,KPIs!B:C,2,0)</f>
         <v>43475</v>
       </c>
@@ -5026,22 +4922,22 @@
       <c r="E4" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="12" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="18" t="n">
+      <c r="I4" s="27"/>
+      <c r="J4" s="12" t="n">
         <v>2</v>
       </c>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="12" t="s">
         <v>81</v>
       </c>
     </row>
@@ -5049,56 +4945,56 @@
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="11" t="n">
         <v>43505</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="20" t="s">
         <v>95</v>
       </c>
       <c r="H5" s="0"/>
-      <c r="I5" s="30" t="n">
+      <c r="I5" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="24"/>
+      <c r="M5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="11" t="n">
         <f aca="false">VLOOKUP(A6,KPIs!B:C,2,0)</f>
         <v>43529</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="20" t="s">
         <v>96</v>
       </c>
       <c r="H6" s="0"/>
-      <c r="I6" s="30" t="n">
+      <c r="I6" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="20" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5130,31 +5026,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="36.062962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="36.9444444444444"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="11" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="22.1481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="12" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="22.637037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="12" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="29" t="s">
         <v>100</v>
       </c>
       <c r="G1" s="0"/>
@@ -5163,20 +5059,20 @@
       <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="B2" s="11" t="n">
         <f aca="false">VLOOKUP(A2,KPIs!B:C,2,0)</f>
         <v>43466</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="17" t="n">
+      <c r="E2" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="10" t="n">
         <v>6</v>
       </c>
       <c r="G2" s="0"/>
@@ -5185,23 +5081,23 @@
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="11" t="n">
         <f aca="false">VLOOKUP(A3,KPIs!B:C,2,0)</f>
         <v>43499</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="17" t="n">
+      <c r="E3" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="17" t="n">
+      <c r="F3" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5221,107 +5117,107 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="42.6259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="24" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="24" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="24" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="24" width="76.0444444444445"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="24" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="1023" min="12" style="24" width="9.11481481481482"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="43.7037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="34.4925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="21" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="77.9037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="21" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1023" min="12" style="21" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="25" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="B2" s="11" t="n">
         <f aca="false">VLOOKUP(A2,KPIs!B:C,2,0)</f>
         <v>43471</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="22" t="n">
+      <c r="B3" s="19" t="n">
         <f aca="false">VLOOKUP(A3,KPIs!B:C,2,0)</f>
         <v>43502</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>75</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -5329,71 +5225,71 @@
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="21" t="s">
         <v>75</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="K3" s="30" t="n">
+      <c r="K3" s="27" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="22" t="n">
+      <c r="B4" s="19" t="n">
         <v>43528</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="11" t="n">
         <f aca="false">VLOOKUP(A5,KPIs!B:C,2,0)</f>
         <v>43559</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="20" t="s">
         <v>110</v>
       </c>
     </row>
@@ -5415,207 +5311,207 @@
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="31.2592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="17.8666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="17.5740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="19.2518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="24" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="24" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="24" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="24" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="24" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="35" width="76.0444444444445"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="36" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="24" width="52.1333333333333"/>
-    <col collapsed="false" hidden="false" max="1022" min="15" style="24" width="9.11481481481482"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="32.0444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="19" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="34.4925925925926"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="21" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="21" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="31" width="77.9037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="21" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="21" width="53.4074074074074"/>
+    <col collapsed="false" hidden="false" max="1022" min="15" style="21" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.31111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="38" t="s">
+      <c r="M1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="25" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22" t="n">
+      <c r="B2" s="19" t="n">
         <f aca="false">VLOOKUP(A2,KPIs!B:C,2,0)</f>
         <v>43467</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>69</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="10" t="s">
         <v>75</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="36" t="n">
+      <c r="M2" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="33" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="22" t="n">
+      <c r="B3" s="19" t="n">
         <f aca="false">VLOOKUP(A3,KPIs!B:C,2,0)</f>
         <v>43468</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="21" t="s">
         <v>117</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="21" t="s">
         <v>117</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
-      <c r="M3" s="36" t="n">
+      <c r="M3" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="30"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="22" t="n">
+      <c r="B4" s="19" t="n">
         <f aca="false">VLOOKUP(A4,KPIs!B:C,2,0)</f>
         <v>43526</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="21" t="s">
         <v>67</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="10" t="s">
         <v>75</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="M4" s="36" t="n">
+      <c r="M4" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="N4" s="30"/>
+      <c r="N4" s="27"/>
     </row>
     <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="19" t="n">
         <f aca="false">VLOOKUP(A5,KPIs!B:C,2,0)</f>
         <v>43557</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="10" t="s">
         <v>75</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="M5" s="36" t="n">
+      <c r="M5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="N5" s="30"/>
+      <c r="N5" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5635,29 +5531,29 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="42.0407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="24.2888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="25.7666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="17" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="17" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="17" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="19.1555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="18" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="43.0185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="4.01851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="16" width="26.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="10" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="10" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="10" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="12" width="27.6333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,7 +5578,7 @@
       <c r="G1" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="34" t="s">
         <v>106</v>
       </c>
       <c r="I1" s="15" t="s">
@@ -5694,7 +5590,7 @@
       <c r="K1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="35" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5702,110 +5598,113 @@
       <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="21" t="n">
+      <c r="B2" s="11" t="n">
         <f aca="false">VLOOKUP(A2,KPIs!B:C,2,0)</f>
         <v>43469</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="10" t="s">
         <v>67</v>
       </c>
       <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
       <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
-      <c r="K2" s="17" t="s">
-        <v>120</v>
+      <c r="K2" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="11" t="n">
         <f aca="false">VLOOKUP(A3,KPIs!B:C,2,0)</f>
         <v>43503</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="10" t="s">
         <v>120</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>120</v>
+      <c r="K3" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="L3" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="11" t="n">
         <f aca="false">VLOOKUP(A4,KPIs!B:C,2,0)</f>
         <v>43527</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="10" t="s">
         <v>67</v>
       </c>
       <c r="G4" s="0"/>
-      <c r="K4" s="17" t="s">
-        <v>120</v>
+      <c r="H4" s="0"/>
+      <c r="K4" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="122.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="11" t="n">
         <f aca="false">VLOOKUP(A5,KPIs!B:C,2,0)</f>
         <v>43558</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="10" t="s">
         <v>120</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>120</v>
+      <c r="K5" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>113</v>

</xml_diff>